<commit_message>
AddPavilionUserControl App.CurrentEmployee EnumerableExtentions TenantInfo PavilionsDbCotext Tests
</commit_message>
<xml_diff>
--- a/Libs/PavilionsData/Resources/Excels/Rentals.xlsx
+++ b/Libs/PavilionsData/Resources/Excels/Rentals.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Id_Rental</t>
   </si>
@@ -47,6 +47,9 @@
   <si>
     <t>RecordStatus</t>
   </si>
+  <si>
+    <t>AdditionalInfo</t>
+  </si>
 </sst>
 </file>
 
@@ -55,13 +58,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,12 +94,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -370,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="M17" activeCellId="1" sqref="N37 M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,7 +396,7 @@
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,11 +421,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -438,7 +454,7 @@
         <v>44152</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -464,7 +480,7 @@
         <v>43939</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -490,7 +506,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -516,7 +532,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -542,7 +558,7 @@
         <v>44008</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -568,7 +584,7 @@
         <v>44170</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -594,7 +610,7 @@
         <v>44120</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -620,7 +636,7 @@
         <v>43740</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -646,7 +662,7 @@
         <v>44009</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -672,7 +688,7 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -698,7 +714,7 @@
         <v>43908</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -724,7 +740,7 @@
         <v>44002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -750,7 +766,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -776,7 +792,7 @@
         <v>44029</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>